<commit_message>
adding new bleu and rouge logic, and new bleu xlsx
</commit_message>
<xml_diff>
--- a/evaluation_results.xlsx
+++ b/evaluation_results.xlsx
@@ -91,47 +91,53 @@
     <t>Simulate the dynamic operation of the electric system, generally on a least-cost system dispatch</t>
   </si>
   <si>
-    <t xml:space="preserve"> Megawatt (MW) is a measure of power, or rate of energy flow, typically used for electric power in watts (W). On the other hand, Megawatt-hour (MWh) is a measure of energy, representing the amount of energy delivered over one hour at a rate of one megawatt. So, 1 MWh is equal to the energy supplied by 1 MW operating for one hour.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Annual Energy Outlook is prepared by the U.S. Department of Energy’s Energy Information Administration (EIA).</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Clean Air Act (CAA) is a U.S. law that defines the Environmental Protection Agency's responsibilities for protecting and improving the nation's air quality and the stratospheric ozone layer. It was last significantly amended in 1990, with minor changes made since then. The CAA sets National Ambient Air Quality Standards for six common air pollutants known as criteria air pollutants, which include particle pollution, ground-level ozone, carbon monoxide, sulfur oxides, nitrogen oxides, and lead.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> An Electric Generating Unit (EGU) refers to a facility that converts energy into electrical power, typically by using a prime mover (such as a gas turbine, steam turbine, or hydro turbine) to spin a generator. The electricity produced can be distributed to various users and loads through the power grid. In some contexts, an EGU may also include renewable energy sources such as wind turbines, solar panels, or biomass generators.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity Dispatch Models optimize the dispatch of a system by simulating the dynamic operation of the electric system on a least-cost system dispatch basis. These models optimize the dispatch of the system based on the variable costs of each resource and any operational constraints that have been entered into the model. They are helpful in assessing which existing plants are displaced, and they are used in short-term planning and regulatory support.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The U.S. Environmental Protection Agency maintains the Emissions &amp; Generation Resource Integrated Database.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Examples of energy efficiency policies include:
-1. Building codes that require energy-efficient construction materials and appliances in new buildings.
-2. Incentives for homeowners to install energy-efficient windows, insulation, or solar panels.
-3. Standards for energy efficiency in industrial equipment, such as motors, pumps, and lighting systems.
-4. Energy Star labels on appliances that meet specific energy efficiency standards.
-5. Policies that encourage the use of public transportation, carpooling, or electric vehicles to reduce energy consumption associated with personal transportation.
-6. Smart grid technologies that improve the management of electricity distribution and reduce losses.
-7. Energy-saving programs for businesses, such as providing rebates for energy-efficient equipment upgrades or implementing energy audits to identify areas for improvement.
-8. Energy efficiency training and education programs for consumers to help them make more informed decisions about energy use in their homes and daily lives.
-9. Policies that promote the adoption of renewable energy sources, such as solar panels or wind turbines, which are often more energy-efficient than traditional fossil fuel power plants.
-10. Energy conservation initiatives, such as turning off lights when not in use, adjusting thermostats to conserve energy during certain hours, or using power strips to minimize energy waste from electronic devices.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In the context provided, ISOs (Independent System Operators) are not explicitly defined. However, in the energy sector, an Independent System Operator is a non-profit organization that manages the transmission of electricity on a regional electric grid. They ensure the reliable operation of the power system and facilitate the wholesale buying and selling of electrical energy and ancillary services. This definition is derived from the context provided, as there are mentions of "electric generating units" and "electricity dispatch models."</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Power pools, also known as Regional Transmission Organizations (RTO) or Independent System Operators (ISO), are organizations responsible for managing the flow of electric power in a region. They operate the high-voltage grid and ensure that electricity is generated, transmitted, and distributed efficiently and reliably. These organizations facilitate the trading of electricity among their members, set rules for operating the grid, and maintain the balance between supply and demand. Power pools help to optimize the use of resources, reduce costs, and enhance the reliability of the power system in their respective regions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Public Utilities Commission (PUC) or Public Service Commission (PSC) is a regulatory body that oversees the utility industries, such as electricity, natural gas, and sometimes telecommunications. They are responsible for ensuring fair and reasonable rates for consumers, promoting competition within the industry, and maintaining reliable service while also considering public safety and environmental concerns. Their roles may include setting regulations, monitoring compliance, resolving disputes between utilities and customers, and encouraging energy efficiency and sustainable practices within the utility sector.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity Dispatch Models simulate the dynamic operation of the electric system, generally on a least-cost system dispatch. These models optimize the dispatch of the system based on the variable costs of each resource and any operational constraints that have been entered into the model. They are helpful in assessing which existing plants are displaced. These models are also used in short-term planning and regulatory support.</t>
+    <t xml:space="preserve"> A Megawatt (MW) measures power, or the rate of energy consumption per unit time. On the other hand, a Megawatt-hour (MWh) is a measure of energy, specifically, one megawatt being sustained for one hour. In simple terms, 1 MW is the amount of power needed to light 1000 100-watt light bulbs continuously for an hour. So, 1 MWh represents the energy equivalent of running 1 MW for one hour.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Annual Energy Outlook was not specifically mentioned in the provided text. It is a report published by the U.S. Energy Information Administration (EIA), which provides projections of energy supply, demand, and prices for the next 25-30 years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Clean Air Act is a legislation in the United States that requires the U.S. Environmental Protection Agency to set National Ambient Air Quality Standards for six common air pollutants. These pollutants are particle pollution, ground-level ozone, carbon monoxide, sulfur oxides, nitrogen oxides, and lead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An Electric Generating Unit (EGU) refers to any facility that produces electricity through the conversion of energy from various sources, such as fossil fuels, nuclear power, or renewable resources like solar, wind, ocean thermal, wave action, and tidal action. In the context provided, it specifically refers to a facility burning fossil fuel and is used in discussions related to reducing emissions and improving air quality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Electricity Dispatch Models (EDMs) optimize the dispatch of a power system by determining the optimal operating conditions for generating units in real-time or near real-time to meet demand and ensure grid stability. They consider multiple factors, including:
+1. Load forecasts: Accurate predictions of electricity consumption are essential for proper dispatch. Load forecasting accounts for weather conditions, time of day, holidays, and other factors that can affect energy demand.
+2. Generation availability: EDMs take into account the current operational status of generators, including maintenance schedules, fuel supply, and outages.
+3. Generator characteristics: The unique technical specifications of each generating unit, such as minimum/maximum output limits, ramp rates, and efficiency levels, are also considered by EDMs to ensure that they operate within their optimal range.
+4. Market pricing signals: Real-time energy market prices can affect the economic dispatch of power plants. For example, generators may prioritize running when prices are high or curtail production when prices are low.
+5. Grid constraints: EDMs must also consider transmission line limitations, such as congestion, voltage limits, and capacity factors to ensure that power flows efficiently and safely within the grid.
+6. Emission targets: To minimize emissions, EDMs can prioritize dispatching cleaner generating units, like renewable energy sources, and optimize their output.
+7. Operating reserve requirements: Reserve margins are necessary to maintain grid reliability and stability in case of unexpected events such as generator outages or sudden changes in load. EDMs must ensure there is an adequate level of reserves available for contingencies.
+In summary, EDMs optimize the dispatch of a power system by balancing electricity demand with available generation while considering a range of operational, market, and grid constraints to maintain reliability, stability, and emissions compliance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Emissions &amp; Generation Resource Integrated Database is maintained by the U.S. Environmental Protection Agency (EPA).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Examples of Energy Efficiency policies, programs and projects include:
+1. Building codes that require energy-efficient construction materials and designs for new buildings.
+2. Appliance standards that set minimum efficiency requirements for appliances such as refrigerators, air conditioners, and lighting fixtures.
+3. Lighting retrofit programs that replace inefficient incandescent bulbs with more efficient compact fluorescent or LED bulbs.
+4. Energy-efficient product labeling programs that help consumers make informed choices about energy-efficient products.
+5. Utility demand-response programs that reduce electricity use during peak demand periods by offering financial incentives to customers who reduce their electricity consumption.
+6. Industrial process optimization programs that identify and implement energy efficiency measures in manufacturing processes.
+7. Energy-efficient transportation programs such as electric vehicles, carpooling, and bike sharing initiatives.
+8. Smart grid technologies that optimize the use of electricity across the power grid to improve efficiency and reduce waste.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In the context provided, there is no definition or mention of "ISOs" (Interconnection System Operators). However, if you're referring to International Organization for Standardization (ISO), it's an independent, non-governmental international organization with a membership of 164 national standards bodies. ISO is responsible for developing and publishing a wide range of standards related to various industries and sectors. These standards aim to provide guidelines and specifications for products, services, and systems, ensuring quality, safety, efficiency, and compatibility.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Based on the provided text, there is no direct mention of "Power Pools" in the context given. Power pools are usually regional organizations that coordinate and manage electricity generation and transmission across multiple utilities to maintain a stable power grid. They operate on the principle of sharing resources and balancing supply and demand. However, without additional context or information, I cannot confidently say if this term is relevant to the text provided.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Public Utilities Commission (PUC) or Public Service Commission (PSC), depending on the state, is a regulatory body that oversees utilities such as electricity, natural gas, water, and sometimes telecommunications. They are responsible for setting rates, rules, and regulations to ensure fair prices, reliable service, safety, and sustainability within the energy sector. In some cases, they may also play a role in promoting renewable energy through policies like Renewable Portfolio Standards or implementing energy efficiency programs. However, specific roles and responsibilities can vary by state.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Electricity Dispatch Models simulate the operation of a power system, including the generation, transmission, and distribution of electricity from various energy sources such as wind, solar, fossil fuels, etc., to meet the demand of consumers at any given time. These models take into account factors like weather conditions (for renewable energy sources), fuel prices, maintenance schedules for power plants, and demand forecasts. They help in optimizing the use of available resources, minimizing operational costs, maintaining grid stability, and meeting regulatory requirements such as Renewable Portfolio Standards.</t>
   </si>
 </sst>
 </file>

</xml_diff>